<commit_message>
new model versions testing for cointegration between stocks and exchange rates in Brasil
</commit_message>
<xml_diff>
--- a/macroeconometrics_i/assignment_1/ibov_data.xlsx
+++ b/macroeconometrics_i/assignment_1/ibov_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrieldiasmp/Documents/pasta_gabriel/codigo/econometrics/macroeconometrics_i/assignment_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FED71580-E8BE-7545-B3D9-8D0B35A1E547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{29BBBDB1-0DD8-6044-A206-30FED9EA97D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="^BVSP (1)" sheetId="1" r:id="rId1"/>
@@ -25,927 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="308" uniqueCount="308">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Close</t>
-  </si>
-  <si>
-    <t>10197.000000</t>
-  </si>
-  <si>
-    <t>9720.000000</t>
-  </si>
-  <si>
-    <t>10571.000000</t>
-  </si>
-  <si>
-    <t>11947.000000</t>
-  </si>
-  <si>
-    <t>11677.000000</t>
-  </si>
-  <si>
-    <t>9847.000000</t>
-  </si>
-  <si>
-    <t>9678.000000</t>
-  </si>
-  <si>
-    <t>10707.000000</t>
-  </si>
-  <si>
-    <t>6472.000000</t>
-  </si>
-  <si>
-    <t>6593.000000</t>
-  </si>
-  <si>
-    <t>7047.000000</t>
-  </si>
-  <si>
-    <t>8631.000000</t>
-  </si>
-  <si>
-    <t>6784.000000</t>
-  </si>
-  <si>
-    <t>8172.000000</t>
-  </si>
-  <si>
-    <t>8911.000000</t>
-  </si>
-  <si>
-    <t>10696.000000</t>
-  </si>
-  <si>
-    <t>11351.000000</t>
-  </si>
-  <si>
-    <t>11090.000000</t>
-  </si>
-  <si>
-    <t>11627.000000</t>
-  </si>
-  <si>
-    <t>10442.000000</t>
-  </si>
-  <si>
-    <t>10565.000000</t>
-  </si>
-  <si>
-    <t>11106.000000</t>
-  </si>
-  <si>
-    <t>11700.000000</t>
-  </si>
-  <si>
-    <t>13779.000000</t>
-  </si>
-  <si>
-    <t>17092.000000</t>
-  </si>
-  <si>
-    <t>16388.000000</t>
-  </si>
-  <si>
-    <t>17660.000000</t>
-  </si>
-  <si>
-    <t>17820.000000</t>
-  </si>
-  <si>
-    <t>15538.000000</t>
-  </si>
-  <si>
-    <t>14957.000000</t>
-  </si>
-  <si>
-    <t>16728.000000</t>
-  </si>
-  <si>
-    <t>16455.000000</t>
-  </si>
-  <si>
-    <t>17347.000000</t>
-  </si>
-  <si>
-    <t>15928.000000</t>
-  </si>
-  <si>
-    <t>14867.000000</t>
-  </si>
-  <si>
-    <t>13287.000000</t>
-  </si>
-  <si>
-    <t>15259.000000</t>
-  </si>
-  <si>
-    <t>15174.000000</t>
-  </si>
-  <si>
-    <t>17673.000000</t>
-  </si>
-  <si>
-    <t>15891.000000</t>
-  </si>
-  <si>
-    <t>14438.000000</t>
-  </si>
-  <si>
-    <t>14918.000000</t>
-  </si>
-  <si>
-    <t>14650.000000</t>
-  </si>
-  <si>
-    <t>14560.000000</t>
-  </si>
-  <si>
-    <t>13754.000000</t>
-  </si>
-  <si>
-    <t>12841.000000</t>
-  </si>
-  <si>
-    <t>10636.000000</t>
-  </si>
-  <si>
-    <t>11365.000000</t>
-  </si>
-  <si>
-    <t>12932.000000</t>
-  </si>
-  <si>
-    <t>13578.000000</t>
-  </si>
-  <si>
-    <t>12721.000000</t>
-  </si>
-  <si>
-    <t>14033.000000</t>
-  </si>
-  <si>
-    <t>13255.000000</t>
-  </si>
-  <si>
-    <t>13085.000000</t>
-  </si>
-  <si>
-    <t>12861.000000</t>
-  </si>
-  <si>
-    <t>11139.000000</t>
-  </si>
-  <si>
-    <t>9763.000000</t>
-  </si>
-  <si>
-    <t>10382.000000</t>
-  </si>
-  <si>
-    <t>8623.000000</t>
-  </si>
-  <si>
-    <t>10168.000000</t>
-  </si>
-  <si>
-    <t>10509.000000</t>
-  </si>
-  <si>
-    <t>11268.000000</t>
-  </si>
-  <si>
-    <t>10941.000000</t>
-  </si>
-  <si>
-    <t>10281.000000</t>
-  </si>
-  <si>
-    <t>11274.000000</t>
-  </si>
-  <si>
-    <t>12557.000000</t>
-  </si>
-  <si>
-    <t>13422.000000</t>
-  </si>
-  <si>
-    <t>12973.000000</t>
-  </si>
-  <si>
-    <t>13572.000000</t>
-  </si>
-  <si>
-    <t>16011.000000</t>
-  </si>
-  <si>
-    <t>17982.000000</t>
-  </si>
-  <si>
-    <t>20184.000000</t>
-  </si>
-  <si>
-    <t>22236.000000</t>
-  </si>
-  <si>
-    <t>21851.000000</t>
-  </si>
-  <si>
-    <t>21755.000000</t>
-  </si>
-  <si>
-    <t>22142.000000</t>
-  </si>
-  <si>
-    <t>19607.000000</t>
-  </si>
-  <si>
-    <t>19545.000000</t>
-  </si>
-  <si>
-    <t>21149.000000</t>
-  </si>
-  <si>
-    <t>22337.000000</t>
-  </si>
-  <si>
-    <t>22803.000000</t>
-  </si>
-  <si>
-    <t>23245.000000</t>
-  </si>
-  <si>
-    <t>23052.000000</t>
-  </si>
-  <si>
-    <t>25128.000000</t>
-  </si>
-  <si>
-    <t>26196.000000</t>
-  </si>
-  <si>
-    <t>24351.000000</t>
-  </si>
-  <si>
-    <t>28139.000000</t>
-  </si>
-  <si>
-    <t>26611.000000</t>
-  </si>
-  <si>
-    <t>24844.000000</t>
-  </si>
-  <si>
-    <t>25207.000000</t>
-  </si>
-  <si>
-    <t>25051.000000</t>
-  </si>
-  <si>
-    <t>26042.000000</t>
-  </si>
-  <si>
-    <t>28045.000000</t>
-  </si>
-  <si>
-    <t>31584.000000</t>
-  </si>
-  <si>
-    <t>30194.000000</t>
-  </si>
-  <si>
-    <t>31917.000000</t>
-  </si>
-  <si>
-    <t>33456.000000</t>
-  </si>
-  <si>
-    <t>38383.000000</t>
-  </si>
-  <si>
-    <t>38610.000000</t>
-  </si>
-  <si>
-    <t>37952.000000</t>
-  </si>
-  <si>
-    <t>40363.000000</t>
-  </si>
-  <si>
-    <t>36530.000000</t>
-  </si>
-  <si>
-    <t>36631.000000</t>
-  </si>
-  <si>
-    <t>37077.000000</t>
-  </si>
-  <si>
-    <t>36232.000000</t>
-  </si>
-  <si>
-    <t>36449.000000</t>
-  </si>
-  <si>
-    <t>39263.000000</t>
-  </si>
-  <si>
-    <t>41932.000000</t>
-  </si>
-  <si>
-    <t>44474.000000</t>
-  </si>
-  <si>
-    <t>44642.000000</t>
-  </si>
-  <si>
-    <t>43892.000000</t>
-  </si>
-  <si>
-    <t>45805.000000</t>
-  </si>
-  <si>
-    <t>48956.000000</t>
-  </si>
-  <si>
-    <t>52268.000000</t>
-  </si>
-  <si>
-    <t>54392.000000</t>
-  </si>
-  <si>
-    <t>54183.000000</t>
-  </si>
-  <si>
-    <t>54637.000000</t>
-  </si>
-  <si>
-    <t>60465.000000</t>
-  </si>
-  <si>
-    <t>65318.000000</t>
-  </si>
-  <si>
-    <t>63006.000000</t>
-  </si>
-  <si>
-    <t>63886.000000</t>
-  </si>
-  <si>
-    <t>59490.000000</t>
-  </si>
-  <si>
-    <t>63489.000000</t>
-  </si>
-  <si>
-    <t>60968.000000</t>
-  </si>
-  <si>
-    <t>67868.000000</t>
-  </si>
-  <si>
-    <t>72593.000000</t>
-  </si>
-  <si>
-    <t>65018.000000</t>
-  </si>
-  <si>
-    <t>59505.000000</t>
-  </si>
-  <si>
-    <t>55680.000000</t>
-  </si>
-  <si>
-    <t>49541.000000</t>
-  </si>
-  <si>
-    <t>37257.000000</t>
-  </si>
-  <si>
-    <t>36596.000000</t>
-  </si>
-  <si>
-    <t>37550.000000</t>
-  </si>
-  <si>
-    <t>39301.000000</t>
-  </si>
-  <si>
-    <t>38183.000000</t>
-  </si>
-  <si>
-    <t>40926.000000</t>
-  </si>
-  <si>
-    <t>47290.000000</t>
-  </si>
-  <si>
-    <t>53198.000000</t>
-  </si>
-  <si>
-    <t>51465.000000</t>
-  </si>
-  <si>
-    <t>54766.000000</t>
-  </si>
-  <si>
-    <t>56489.000000</t>
-  </si>
-  <si>
-    <t>61518.000000</t>
-  </si>
-  <si>
-    <t>67530.000000</t>
-  </si>
-  <si>
-    <t>61546.000000</t>
-  </si>
-  <si>
-    <t>67044.000000</t>
-  </si>
-  <si>
-    <t>68588.000000</t>
-  </si>
-  <si>
-    <t>68587.000000</t>
-  </si>
-  <si>
-    <t>65402.000000</t>
-  </si>
-  <si>
-    <t>66503.000000</t>
-  </si>
-  <si>
-    <t>70372.000000</t>
-  </si>
-  <si>
-    <t>63047.000000</t>
-  </si>
-  <si>
-    <t>60936.000000</t>
-  </si>
-  <si>
-    <t>67515.000000</t>
-  </si>
-  <si>
-    <t>65145.000000</t>
-  </si>
-  <si>
-    <t>69430.000000</t>
-  </si>
-  <si>
-    <t>70673.000000</t>
-  </si>
-  <si>
-    <t>67705.000000</t>
-  </si>
-  <si>
-    <t>69305.000000</t>
-  </si>
-  <si>
-    <t>66575.000000</t>
-  </si>
-  <si>
-    <t>67383.000000</t>
-  </si>
-  <si>
-    <t>66133.000000</t>
-  </si>
-  <si>
-    <t>64620.000000</t>
-  </si>
-  <si>
-    <t>62404.000000</t>
-  </si>
-  <si>
-    <t>58823.000000</t>
-  </si>
-  <si>
-    <t>56495.000000</t>
-  </si>
-  <si>
-    <t>52324.000000</t>
-  </si>
-  <si>
-    <t>58338.000000</t>
-  </si>
-  <si>
-    <t>56875.000000</t>
-  </si>
-  <si>
-    <t>56754.000000</t>
-  </si>
-  <si>
-    <t>63072.000000</t>
-  </si>
-  <si>
-    <t>66662.000000</t>
-  </si>
-  <si>
-    <t>65812.000000</t>
-  </si>
-  <si>
-    <t>64511.000000</t>
-  </si>
-  <si>
-    <t>61820.000000</t>
-  </si>
-  <si>
-    <t>54490.000000</t>
-  </si>
-  <si>
-    <t>54355.000000</t>
-  </si>
-  <si>
-    <t>56097.000000</t>
-  </si>
-  <si>
-    <t>57061.000000</t>
-  </si>
-  <si>
-    <t>59176.000000</t>
-  </si>
-  <si>
-    <t>57068.000000</t>
-  </si>
-  <si>
-    <t>57475.000000</t>
-  </si>
-  <si>
-    <t>60952.000000</t>
-  </si>
-  <si>
-    <t>59761.000000</t>
-  </si>
-  <si>
-    <t>57424.000000</t>
-  </si>
-  <si>
-    <t>56352.000000</t>
-  </si>
-  <si>
-    <t>55910.000000</t>
-  </si>
-  <si>
-    <t>53506.000000</t>
-  </si>
-  <si>
-    <t>47457.000000</t>
-  </si>
-  <si>
-    <t>48234.000000</t>
-  </si>
-  <si>
-    <t>50008.000000</t>
-  </si>
-  <si>
-    <t>52338.000000</t>
-  </si>
-  <si>
-    <t>54256.000000</t>
-  </si>
-  <si>
-    <t>52482.000000</t>
-  </si>
-  <si>
-    <t>51507.000000</t>
-  </si>
-  <si>
-    <t>47639.000000</t>
-  </si>
-  <si>
-    <t>47094.000000</t>
-  </si>
-  <si>
-    <t>50415.000000</t>
-  </si>
-  <si>
-    <t>51626.000000</t>
-  </si>
-  <si>
-    <t>51239.000000</t>
-  </si>
-  <si>
-    <t>53168.000000</t>
-  </si>
-  <si>
-    <t>55829.000000</t>
-  </si>
-  <si>
-    <t>61288.000000</t>
-  </si>
-  <si>
-    <t>54116.000000</t>
-  </si>
-  <si>
-    <t>54629.000000</t>
-  </si>
-  <si>
-    <t>54664.000000</t>
-  </si>
-  <si>
-    <t>50007.000000</t>
-  </si>
-  <si>
-    <t>46908.000000</t>
-  </si>
-  <si>
-    <t>51583.000000</t>
-  </si>
-  <si>
-    <t>51150.000000</t>
-  </si>
-  <si>
-    <t>56229.000000</t>
-  </si>
-  <si>
-    <t>52760.000000</t>
-  </si>
-  <si>
-    <t>53081.000000</t>
-  </si>
-  <si>
-    <t>50865.000000</t>
-  </si>
-  <si>
-    <t>46626.000000</t>
-  </si>
-  <si>
-    <t>45059.000000</t>
-  </si>
-  <si>
-    <t>45869.000000</t>
-  </si>
-  <si>
-    <t>45120.000000</t>
-  </si>
-  <si>
-    <t>43350.000000</t>
-  </si>
-  <si>
-    <t>40406.000000</t>
-  </si>
-  <si>
-    <t>42794.000000</t>
-  </si>
-  <si>
-    <t>50055.000000</t>
-  </si>
-  <si>
-    <t>53911.000000</t>
-  </si>
-  <si>
-    <t>48472.000000</t>
-  </si>
-  <si>
-    <t>51527.000000</t>
-  </si>
-  <si>
-    <t>57308.000000</t>
-  </si>
-  <si>
-    <t>57901.000000</t>
-  </si>
-  <si>
-    <t>58367.000000</t>
-  </si>
-  <si>
-    <t>64925.000000</t>
-  </si>
-  <si>
-    <t>61906.000000</t>
-  </si>
-  <si>
-    <t>60227.000000</t>
-  </si>
-  <si>
-    <t>64671.000000</t>
-  </si>
-  <si>
-    <t>64984.000000</t>
-  </si>
-  <si>
-    <t>65403.000000</t>
-  </si>
-  <si>
-    <t>62711.000000</t>
-  </si>
-  <si>
-    <t>62900.000000</t>
-  </si>
-  <si>
-    <t>65920.000000</t>
-  </si>
-  <si>
-    <t>70835.000000</t>
-  </si>
-  <si>
-    <t>74294.000000</t>
-  </si>
-  <si>
-    <t>74308.000000</t>
-  </si>
-  <si>
-    <t>71971.000000</t>
-  </si>
-  <si>
-    <t>76402.000000</t>
-  </si>
-  <si>
-    <t>84913.000000</t>
-  </si>
-  <si>
-    <t>85481.000000</t>
-  </si>
-  <si>
-    <t>85366.000000</t>
-  </si>
-  <si>
-    <t>86115.000000</t>
-  </si>
-  <si>
-    <t>76754.000000</t>
-  </si>
-  <si>
-    <t>72763.000000</t>
-  </si>
-  <si>
-    <t>79220.000000</t>
-  </si>
-  <si>
-    <t>76678.000000</t>
-  </si>
-  <si>
-    <t>79342.000000</t>
-  </si>
-  <si>
-    <t>87424.000000</t>
-  </si>
-  <si>
-    <t>89504.000000</t>
-  </si>
-  <si>
-    <t>87887.000000</t>
-  </si>
-  <si>
-    <t>97394.000000</t>
-  </si>
-  <si>
-    <t>95584.000000</t>
-  </si>
-  <si>
-    <t>95415.000000</t>
-  </si>
-  <si>
-    <t>96353.000000</t>
-  </si>
-  <si>
-    <t>97030.000000</t>
-  </si>
-  <si>
-    <t>100967.000000</t>
-  </si>
-  <si>
-    <t>101812.000000</t>
-  </si>
-  <si>
-    <t>101135.000000</t>
-  </si>
-  <si>
-    <t>104745.000000</t>
-  </si>
-  <si>
-    <t>107220.000000</t>
-  </si>
-  <si>
-    <t>108233.000000</t>
-  </si>
-  <si>
-    <t>115645.000000</t>
-  </si>
-  <si>
-    <t>113761.000000</t>
-  </si>
-  <si>
-    <t>104172.000000</t>
-  </si>
-  <si>
-    <t>73020.000000</t>
-  </si>
-  <si>
-    <t>80506.000000</t>
-  </si>
-  <si>
-    <t>87403.000000</t>
-  </si>
-  <si>
-    <t>95056.000000</t>
-  </si>
-  <si>
-    <t>102912.000000</t>
-  </si>
-  <si>
-    <t>99369.000000</t>
-  </si>
-  <si>
-    <t>94603.000000</t>
-  </si>
-  <si>
-    <t>93952.000000</t>
-  </si>
-  <si>
-    <t>108888.000000</t>
-  </si>
-  <si>
-    <t>119306.000000</t>
-  </si>
-  <si>
-    <t>116007.000000</t>
-  </si>
-  <si>
-    <t>110035.000000</t>
-  </si>
-  <si>
-    <t>116634.000000</t>
-  </si>
-  <si>
-    <t>118894.000000</t>
-  </si>
-  <si>
-    <t>126216.000000</t>
-  </si>
-  <si>
-    <t>126802.000000</t>
-  </si>
-  <si>
-    <t>121801.000000</t>
-  </si>
-  <si>
-    <t>118781.000000</t>
-  </si>
-  <si>
-    <t>110979.000000</t>
-  </si>
-  <si>
-    <t>103501.000000</t>
-  </si>
-  <si>
-    <t>101915.000000</t>
-  </si>
-  <si>
-    <t>104822.000000</t>
-  </si>
-  <si>
-    <t>112388.000000</t>
-  </si>
-  <si>
-    <t>113142.000000</t>
-  </si>
-  <si>
-    <t>119999.000000</t>
-  </si>
-  <si>
-    <t>107876.000000</t>
-  </si>
-  <si>
-    <t>111351.000000</t>
-  </si>
-  <si>
-    <t>98542.000000</t>
-  </si>
-  <si>
-    <t>103165.000000</t>
-  </si>
-  <si>
-    <t>109523.000000</t>
-  </si>
-  <si>
-    <t>110037.000000</t>
-  </si>
-  <si>
-    <t>116037.000000</t>
-  </si>
-  <si>
-    <t>112486.000000</t>
-  </si>
-  <si>
-    <t>110031.000000</t>
-  </si>
-  <si>
-    <t>113532.000000</t>
-  </si>
-  <si>
-    <t>104932.000000</t>
-  </si>
-  <si>
-    <t>101793.000000</t>
-  </si>
-  <si>
-    <t>101792.523438</t>
   </si>
   <si>
     <t>ibov_returns</t>
@@ -954,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1789,11 +874,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1806,2447 +891,2447 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>307</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="d">
         <v>1997-12-01</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>10197</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="d">
         <v>1998-01-01</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>9720</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="d">
         <v>1998-02-01</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>10571</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="d">
         <v>1998-03-01</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <v>11947</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="d">
         <v>1998-04-01</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="B6">
+        <v>11677</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="d">
         <v>1998-05-01</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
+      <c r="B7">
+        <v>9847</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="d">
         <v>1998-06-01</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
+      <c r="B8">
+        <v>9678</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="d">
         <v>1998-07-01</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
+      <c r="B9">
+        <v>10707</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="d">
         <v>1998-08-01</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B10">
+        <v>6472</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="d">
         <v>1998-09-01</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="B11">
+        <v>6593</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="d">
         <v>1998-10-01</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
+      <c r="B12">
+        <v>7047</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="d">
         <v>1998-11-01</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
+      <c r="B13">
+        <v>8631</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="d">
         <v>1998-12-01</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
+      <c r="B14">
+        <v>6784</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="d">
         <v>1999-01-01</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
+      <c r="B15">
+        <v>8172</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="d">
         <v>1999-02-01</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
+      <c r="B16">
+        <v>8911</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="d">
         <v>1999-03-01</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
+      <c r="B17">
+        <v>10696</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="d">
         <v>1999-04-01</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
+      <c r="B18">
+        <v>11351</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="d">
         <v>1999-05-01</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
+      <c r="B19">
+        <v>11090</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="d">
         <v>1999-06-01</v>
       </c>
-      <c r="B20" t="s">
-        <v>20</v>
+      <c r="B20">
+        <v>11627</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="d">
         <v>1999-07-01</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
+      <c r="B21">
+        <v>10442</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="d">
         <v>1999-08-01</v>
       </c>
-      <c r="B22" t="s">
-        <v>22</v>
+      <c r="B22">
+        <v>10565</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="d">
         <v>1999-09-01</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
+      <c r="B23">
+        <v>11106</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="d">
         <v>1999-10-01</v>
       </c>
-      <c r="B24" t="s">
-        <v>24</v>
+      <c r="B24">
+        <v>11700</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="d">
         <v>1999-11-01</v>
       </c>
-      <c r="B25" t="s">
-        <v>25</v>
+      <c r="B25">
+        <v>13779</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="d">
         <v>1999-12-01</v>
       </c>
-      <c r="B26" t="s">
-        <v>26</v>
+      <c r="B26">
+        <v>17092</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="d">
         <v>2000-01-01</v>
       </c>
-      <c r="B27" t="s">
-        <v>27</v>
+      <c r="B27">
+        <v>16388</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="d">
         <v>2000-02-01</v>
       </c>
-      <c r="B28" t="s">
-        <v>28</v>
+      <c r="B28">
+        <v>17660</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="d">
         <v>2000-03-01</v>
       </c>
-      <c r="B29" t="s">
-        <v>29</v>
+      <c r="B29">
+        <v>17820</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="d">
         <v>2000-04-01</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
+      <c r="B30">
+        <v>15538</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="d">
         <v>2000-05-01</v>
       </c>
-      <c r="B31" t="s">
-        <v>31</v>
+      <c r="B31">
+        <v>14957</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="d">
         <v>2000-06-01</v>
       </c>
-      <c r="B32" t="s">
-        <v>32</v>
+      <c r="B32">
+        <v>16728</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="d">
         <v>2000-07-01</v>
       </c>
-      <c r="B33" t="s">
-        <v>33</v>
+      <c r="B33">
+        <v>16455</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="d">
         <v>2000-08-01</v>
       </c>
-      <c r="B34" t="s">
-        <v>34</v>
+      <c r="B34">
+        <v>17347</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="d">
         <v>2000-09-01</v>
       </c>
-      <c r="B35" t="s">
-        <v>35</v>
+      <c r="B35">
+        <v>15928</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="d">
         <v>2000-10-01</v>
       </c>
-      <c r="B36" t="s">
-        <v>36</v>
+      <c r="B36">
+        <v>14867</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="d">
         <v>2000-11-01</v>
       </c>
-      <c r="B37" t="s">
-        <v>37</v>
+      <c r="B37">
+        <v>13287</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="d">
         <v>2000-12-01</v>
       </c>
-      <c r="B38" t="s">
-        <v>38</v>
+      <c r="B38">
+        <v>15259</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="d">
         <v>2001-01-01</v>
       </c>
-      <c r="B39" t="s">
-        <v>40</v>
+      <c r="B39">
+        <v>17673</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="d">
         <v>2001-02-01</v>
       </c>
-      <c r="B40" t="s">
-        <v>41</v>
+      <c r="B40">
+        <v>15891</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="d">
         <v>2001-03-01</v>
       </c>
-      <c r="B41" t="s">
-        <v>42</v>
+      <c r="B41">
+        <v>14438</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="d">
         <v>2001-04-01</v>
       </c>
-      <c r="B42" t="s">
-        <v>43</v>
+      <c r="B42">
+        <v>14918</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="d">
         <v>2001-05-01</v>
       </c>
-      <c r="B43" t="s">
-        <v>44</v>
+      <c r="B43">
+        <v>14650</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="d">
         <v>2001-06-01</v>
       </c>
-      <c r="B44" t="s">
-        <v>45</v>
+      <c r="B44">
+        <v>14560</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="d">
         <v>2001-07-01</v>
       </c>
-      <c r="B45" t="s">
-        <v>46</v>
+      <c r="B45">
+        <v>13754</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="d">
         <v>2001-08-01</v>
       </c>
-      <c r="B46" t="s">
-        <v>47</v>
+      <c r="B46">
+        <v>12841</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="d">
         <v>2001-09-01</v>
       </c>
-      <c r="B47" t="s">
-        <v>48</v>
+      <c r="B47">
+        <v>10636</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="d">
         <v>2001-10-01</v>
       </c>
-      <c r="B48" t="s">
-        <v>49</v>
+      <c r="B48">
+        <v>11365</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="d">
         <v>2001-11-01</v>
       </c>
-      <c r="B49" t="s">
-        <v>50</v>
+      <c r="B49">
+        <v>12932</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="d">
         <v>2001-12-01</v>
       </c>
-      <c r="B50" t="s">
-        <v>51</v>
+      <c r="B50">
+        <v>13578</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="d">
         <v>2002-01-01</v>
       </c>
-      <c r="B51" t="s">
-        <v>52</v>
+      <c r="B51">
+        <v>12721</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="d">
         <v>2002-02-01</v>
       </c>
-      <c r="B52" t="s">
-        <v>53</v>
+      <c r="B52">
+        <v>14033</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="d">
         <v>2002-03-01</v>
       </c>
-      <c r="B53" t="s">
-        <v>54</v>
+      <c r="B53">
+        <v>13255</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="d">
         <v>2002-04-01</v>
       </c>
-      <c r="B54" t="s">
-        <v>55</v>
+      <c r="B54">
+        <v>13085</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="d">
         <v>2002-05-01</v>
       </c>
-      <c r="B55" t="s">
-        <v>56</v>
+      <c r="B55">
+        <v>12861</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="d">
         <v>2002-06-01</v>
       </c>
-      <c r="B56" t="s">
-        <v>57</v>
+      <c r="B56">
+        <v>11139</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="d">
         <v>2002-07-01</v>
       </c>
-      <c r="B57" t="s">
-        <v>58</v>
+      <c r="B57">
+        <v>9763</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="d">
         <v>2002-08-01</v>
       </c>
-      <c r="B58" t="s">
-        <v>59</v>
+      <c r="B58">
+        <v>10382</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="d">
         <v>2002-09-01</v>
       </c>
-      <c r="B59" t="s">
-        <v>60</v>
+      <c r="B59">
+        <v>8623</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="d">
         <v>2002-10-01</v>
       </c>
-      <c r="B60" t="s">
-        <v>61</v>
+      <c r="B60">
+        <v>10168</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="d">
         <v>2002-11-01</v>
       </c>
-      <c r="B61" t="s">
-        <v>62</v>
+      <c r="B61">
+        <v>10509</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="d">
         <v>2002-12-01</v>
       </c>
-      <c r="B62" t="s">
-        <v>63</v>
+      <c r="B62">
+        <v>11268</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="d">
         <v>2003-01-01</v>
       </c>
-      <c r="B63" t="s">
-        <v>64</v>
+      <c r="B63">
+        <v>10941</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="d">
         <v>2003-02-01</v>
       </c>
-      <c r="B64" t="s">
-        <v>65</v>
+      <c r="B64">
+        <v>10281</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="d">
         <v>2003-03-01</v>
       </c>
-      <c r="B65" t="s">
-        <v>66</v>
+      <c r="B65">
+        <v>11274</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="d">
         <v>2003-04-01</v>
       </c>
-      <c r="B66" t="s">
-        <v>67</v>
+      <c r="B66">
+        <v>12557</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="d">
         <v>2003-05-01</v>
       </c>
-      <c r="B67" t="s">
-        <v>68</v>
+      <c r="B67">
+        <v>13422</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="d">
         <v>2003-06-01</v>
       </c>
-      <c r="B68" t="s">
-        <v>69</v>
+      <c r="B68">
+        <v>12973</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="d">
         <v>2003-07-01</v>
       </c>
-      <c r="B69" t="s">
-        <v>70</v>
+      <c r="B69">
+        <v>13572</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="d">
         <v>2003-08-01</v>
       </c>
-      <c r="B70" t="s">
-        <v>39</v>
+      <c r="B70">
+        <v>15174</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="d">
         <v>2003-09-01</v>
       </c>
-      <c r="B71" t="s">
-        <v>71</v>
+      <c r="B71">
+        <v>16011</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="d">
         <v>2003-10-01</v>
       </c>
-      <c r="B72" t="s">
-        <v>72</v>
+      <c r="B72">
+        <v>17982</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="d">
         <v>2003-11-01</v>
       </c>
-      <c r="B73" t="s">
-        <v>73</v>
+      <c r="B73">
+        <v>20184</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="d">
         <v>2003-12-01</v>
       </c>
-      <c r="B74" t="s">
-        <v>74</v>
+      <c r="B74">
+        <v>22236</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="d">
         <v>2004-01-01</v>
       </c>
-      <c r="B75" t="s">
-        <v>75</v>
+      <c r="B75">
+        <v>21851</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="d">
         <v>2004-02-01</v>
       </c>
-      <c r="B76" t="s">
-        <v>76</v>
+      <c r="B76">
+        <v>21755</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="d">
         <v>2004-03-01</v>
       </c>
-      <c r="B77" t="s">
-        <v>77</v>
+      <c r="B77">
+        <v>22142</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="d">
         <v>2004-04-01</v>
       </c>
-      <c r="B78" t="s">
-        <v>78</v>
+      <c r="B78">
+        <v>19607</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="d">
         <v>2004-05-01</v>
       </c>
-      <c r="B79" t="s">
-        <v>79</v>
+      <c r="B79">
+        <v>19545</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="d">
         <v>2004-06-01</v>
       </c>
-      <c r="B80" t="s">
-        <v>80</v>
+      <c r="B80">
+        <v>21149</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="d">
         <v>2004-07-01</v>
       </c>
-      <c r="B81" t="s">
-        <v>81</v>
+      <c r="B81">
+        <v>22337</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="d">
         <v>2004-08-01</v>
       </c>
-      <c r="B82" t="s">
-        <v>82</v>
+      <c r="B82">
+        <v>22803</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="d">
         <v>2004-09-01</v>
       </c>
-      <c r="B83" t="s">
-        <v>83</v>
+      <c r="B83">
+        <v>23245</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="d">
         <v>2004-10-01</v>
       </c>
-      <c r="B84" t="s">
-        <v>84</v>
+      <c r="B84">
+        <v>23052</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="d">
         <v>2004-11-01</v>
       </c>
-      <c r="B85" t="s">
-        <v>85</v>
+      <c r="B85">
+        <v>25128</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="d">
         <v>2004-12-01</v>
       </c>
-      <c r="B86" t="s">
-        <v>86</v>
+      <c r="B86">
+        <v>26196</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="d">
         <v>2005-01-01</v>
       </c>
-      <c r="B87" t="s">
-        <v>87</v>
+      <c r="B87">
+        <v>24351</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="d">
         <v>2005-02-01</v>
       </c>
-      <c r="B88" t="s">
-        <v>88</v>
+      <c r="B88">
+        <v>28139</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="d">
         <v>2005-03-01</v>
       </c>
-      <c r="B89" t="s">
-        <v>89</v>
+      <c r="B89">
+        <v>26611</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="d">
         <v>2005-04-01</v>
       </c>
-      <c r="B90" t="s">
-        <v>90</v>
+      <c r="B90">
+        <v>24844</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="d">
         <v>2005-05-01</v>
       </c>
-      <c r="B91" t="s">
-        <v>91</v>
+      <c r="B91">
+        <v>25207</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="d">
         <v>2005-06-01</v>
       </c>
-      <c r="B92" t="s">
-        <v>92</v>
+      <c r="B92">
+        <v>25051</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="d">
         <v>2005-07-01</v>
       </c>
-      <c r="B93" t="s">
-        <v>93</v>
+      <c r="B93">
+        <v>26042</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="d">
         <v>2005-08-01</v>
       </c>
-      <c r="B94" t="s">
-        <v>94</v>
+      <c r="B94">
+        <v>28045</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="d">
         <v>2005-09-01</v>
       </c>
-      <c r="B95" t="s">
-        <v>95</v>
+      <c r="B95">
+        <v>31584</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="d">
         <v>2005-10-01</v>
       </c>
-      <c r="B96" t="s">
-        <v>96</v>
+      <c r="B96">
+        <v>30194</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="d">
         <v>2005-11-01</v>
       </c>
-      <c r="B97" t="s">
-        <v>97</v>
+      <c r="B97">
+        <v>31917</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="d">
         <v>2005-12-01</v>
       </c>
-      <c r="B98" t="s">
-        <v>98</v>
+      <c r="B98">
+        <v>33456</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="d">
         <v>2006-01-01</v>
       </c>
-      <c r="B99" t="s">
-        <v>99</v>
+      <c r="B99">
+        <v>38383</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="d">
         <v>2006-02-01</v>
       </c>
-      <c r="B100" t="s">
-        <v>100</v>
+      <c r="B100">
+        <v>38610</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="d">
         <v>2006-03-01</v>
       </c>
-      <c r="B101" t="s">
-        <v>101</v>
+      <c r="B101">
+        <v>37952</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="d">
         <v>2006-04-01</v>
       </c>
-      <c r="B102" t="s">
-        <v>102</v>
+      <c r="B102">
+        <v>40363</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="d">
         <v>2006-05-01</v>
       </c>
-      <c r="B103" t="s">
-        <v>103</v>
+      <c r="B103">
+        <v>36530</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="d">
         <v>2006-06-01</v>
       </c>
-      <c r="B104" t="s">
-        <v>104</v>
+      <c r="B104">
+        <v>36631</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="d">
         <v>2006-07-01</v>
       </c>
-      <c r="B105" t="s">
-        <v>105</v>
+      <c r="B105">
+        <v>37077</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="d">
         <v>2006-08-01</v>
       </c>
-      <c r="B106" t="s">
-        <v>106</v>
+      <c r="B106">
+        <v>36232</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="d">
         <v>2006-09-01</v>
       </c>
-      <c r="B107" t="s">
-        <v>107</v>
+      <c r="B107">
+        <v>36449</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="d">
         <v>2006-10-01</v>
       </c>
-      <c r="B108" t="s">
-        <v>108</v>
+      <c r="B108">
+        <v>39263</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="d">
         <v>2006-11-01</v>
       </c>
-      <c r="B109" t="s">
-        <v>109</v>
+      <c r="B109">
+        <v>41932</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="d">
         <v>2006-12-01</v>
       </c>
-      <c r="B110" t="s">
-        <v>110</v>
+      <c r="B110">
+        <v>44474</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="d">
         <v>2007-01-01</v>
       </c>
-      <c r="B111" t="s">
-        <v>111</v>
+      <c r="B111">
+        <v>44642</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="d">
         <v>2007-02-01</v>
       </c>
-      <c r="B112" t="s">
-        <v>112</v>
+      <c r="B112">
+        <v>43892</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="d">
         <v>2007-03-01</v>
       </c>
-      <c r="B113" t="s">
-        <v>113</v>
+      <c r="B113">
+        <v>45805</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="d">
         <v>2007-04-01</v>
       </c>
-      <c r="B114" t="s">
-        <v>114</v>
+      <c r="B114">
+        <v>48956</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="d">
         <v>2007-05-01</v>
       </c>
-      <c r="B115" t="s">
-        <v>115</v>
+      <c r="B115">
+        <v>52268</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="d">
         <v>2007-06-01</v>
       </c>
-      <c r="B116" t="s">
-        <v>116</v>
+      <c r="B116">
+        <v>54392</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="d">
         <v>2007-07-01</v>
       </c>
-      <c r="B117" t="s">
-        <v>117</v>
+      <c r="B117">
+        <v>54183</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="d">
         <v>2007-08-01</v>
       </c>
-      <c r="B118" t="s">
-        <v>118</v>
+      <c r="B118">
+        <v>54637</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="d">
         <v>2007-09-01</v>
       </c>
-      <c r="B119" t="s">
-        <v>119</v>
+      <c r="B119">
+        <v>60465</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="d">
         <v>2007-10-01</v>
       </c>
-      <c r="B120" t="s">
-        <v>120</v>
+      <c r="B120">
+        <v>65318</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="d">
         <v>2007-11-01</v>
       </c>
-      <c r="B121" t="s">
-        <v>121</v>
+      <c r="B121">
+        <v>63006</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="d">
         <v>2007-12-01</v>
       </c>
-      <c r="B122" t="s">
-        <v>122</v>
+      <c r="B122">
+        <v>63886</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="d">
         <v>2008-01-01</v>
       </c>
-      <c r="B123" t="s">
-        <v>123</v>
+      <c r="B123">
+        <v>59490</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="d">
         <v>2008-02-01</v>
       </c>
-      <c r="B124" t="s">
-        <v>124</v>
+      <c r="B124">
+        <v>63489</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="d">
         <v>2008-03-01</v>
       </c>
-      <c r="B125" t="s">
-        <v>125</v>
+      <c r="B125">
+        <v>60968</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="d">
         <v>2008-04-01</v>
       </c>
-      <c r="B126" t="s">
-        <v>126</v>
+      <c r="B126">
+        <v>67868</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="d">
         <v>2008-05-01</v>
       </c>
-      <c r="B127" t="s">
-        <v>127</v>
+      <c r="B127">
+        <v>72593</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="d">
         <v>2008-06-01</v>
       </c>
-      <c r="B128" t="s">
-        <v>128</v>
+      <c r="B128">
+        <v>65018</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="d">
         <v>2008-07-01</v>
       </c>
-      <c r="B129" t="s">
-        <v>129</v>
+      <c r="B129">
+        <v>59505</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="d">
         <v>2008-08-01</v>
       </c>
-      <c r="B130" t="s">
-        <v>130</v>
+      <c r="B130">
+        <v>55680</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="d">
         <v>2008-09-01</v>
       </c>
-      <c r="B131" t="s">
-        <v>131</v>
+      <c r="B131">
+        <v>49541</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="d">
         <v>2008-10-01</v>
       </c>
-      <c r="B132" t="s">
-        <v>132</v>
+      <c r="B132">
+        <v>37257</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="d">
         <v>2008-11-01</v>
       </c>
-      <c r="B133" t="s">
-        <v>133</v>
+      <c r="B133">
+        <v>36596</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="d">
         <v>2008-12-01</v>
       </c>
-      <c r="B134" t="s">
-        <v>134</v>
+      <c r="B134">
+        <v>37550</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="d">
         <v>2009-01-01</v>
       </c>
-      <c r="B135" t="s">
-        <v>135</v>
+      <c r="B135">
+        <v>39301</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="d">
         <v>2009-02-01</v>
       </c>
-      <c r="B136" t="s">
-        <v>136</v>
+      <c r="B136">
+        <v>38183</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="d">
         <v>2009-03-01</v>
       </c>
-      <c r="B137" t="s">
-        <v>137</v>
+      <c r="B137">
+        <v>40926</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="d">
         <v>2009-04-01</v>
       </c>
-      <c r="B138" t="s">
-        <v>138</v>
+      <c r="B138">
+        <v>47290</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="d">
         <v>2009-05-01</v>
       </c>
-      <c r="B139" t="s">
-        <v>139</v>
+      <c r="B139">
+        <v>53198</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="d">
         <v>2009-06-01</v>
       </c>
-      <c r="B140" t="s">
-        <v>140</v>
+      <c r="B140">
+        <v>51465</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="d">
         <v>2009-07-01</v>
       </c>
-      <c r="B141" t="s">
-        <v>141</v>
+      <c r="B141">
+        <v>54766</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="d">
         <v>2009-08-01</v>
       </c>
-      <c r="B142" t="s">
-        <v>142</v>
+      <c r="B142">
+        <v>56489</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="d">
         <v>2009-09-01</v>
       </c>
-      <c r="B143" t="s">
-        <v>143</v>
+      <c r="B143">
+        <v>61518</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="d">
         <v>2009-10-01</v>
       </c>
-      <c r="B144" t="s">
-        <v>145</v>
+      <c r="B144">
+        <v>61546</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="d">
         <v>2009-11-01</v>
       </c>
-      <c r="B145" t="s">
-        <v>146</v>
+      <c r="B145">
+        <v>67044</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="d">
         <v>2009-12-01</v>
       </c>
-      <c r="B146" t="s">
-        <v>147</v>
+      <c r="B146">
+        <v>68588</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="d">
         <v>2010-01-01</v>
       </c>
-      <c r="B147" t="s">
-        <v>149</v>
+      <c r="B147">
+        <v>65402</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="d">
         <v>2010-02-01</v>
       </c>
-      <c r="B148" t="s">
-        <v>150</v>
+      <c r="B148">
+        <v>66503</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="d">
         <v>2010-03-01</v>
       </c>
-      <c r="B149" t="s">
-        <v>151</v>
+      <c r="B149">
+        <v>70372</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="d">
         <v>2010-04-01</v>
       </c>
-      <c r="B150" t="s">
-        <v>144</v>
+      <c r="B150">
+        <v>67530</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="d">
         <v>2010-05-01</v>
       </c>
-      <c r="B151" t="s">
-        <v>152</v>
+      <c r="B151">
+        <v>63047</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="d">
         <v>2010-06-01</v>
       </c>
-      <c r="B152" t="s">
-        <v>153</v>
+      <c r="B152">
+        <v>60936</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="d">
         <v>2010-07-01</v>
       </c>
-      <c r="B153" t="s">
-        <v>154</v>
+      <c r="B153">
+        <v>67515</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="d">
         <v>2010-08-01</v>
       </c>
-      <c r="B154" t="s">
-        <v>155</v>
+      <c r="B154">
+        <v>65145</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="d">
         <v>2010-09-01</v>
       </c>
-      <c r="B155" t="s">
-        <v>156</v>
+      <c r="B155">
+        <v>69430</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="d">
         <v>2010-10-01</v>
       </c>
-      <c r="B156" t="s">
-        <v>157</v>
+      <c r="B156">
+        <v>70673</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="d">
         <v>2010-11-01</v>
       </c>
-      <c r="B157" t="s">
-        <v>158</v>
+      <c r="B157">
+        <v>67705</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="d">
         <v>2010-12-01</v>
       </c>
-      <c r="B158" t="s">
-        <v>159</v>
+      <c r="B158">
+        <v>69305</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="d">
         <v>2011-01-01</v>
       </c>
-      <c r="B159" t="s">
-        <v>160</v>
+      <c r="B159">
+        <v>66575</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="d">
         <v>2011-02-01</v>
       </c>
-      <c r="B160" t="s">
-        <v>161</v>
+      <c r="B160">
+        <v>67383</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="d">
         <v>2011-03-01</v>
       </c>
-      <c r="B161" t="s">
-        <v>148</v>
+      <c r="B161">
+        <v>68587</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="d">
         <v>2011-04-01</v>
       </c>
-      <c r="B162" t="s">
-        <v>162</v>
+      <c r="B162">
+        <v>66133</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="d">
         <v>2011-05-01</v>
       </c>
-      <c r="B163" t="s">
-        <v>163</v>
+      <c r="B163">
+        <v>64620</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="d">
         <v>2011-06-01</v>
       </c>
-      <c r="B164" t="s">
-        <v>164</v>
+      <c r="B164">
+        <v>62404</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="d">
         <v>2011-07-01</v>
       </c>
-      <c r="B165" t="s">
-        <v>165</v>
+      <c r="B165">
+        <v>58823</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="d">
         <v>2011-08-01</v>
       </c>
-      <c r="B166" t="s">
-        <v>166</v>
+      <c r="B166">
+        <v>56495</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="d">
         <v>2011-09-01</v>
       </c>
-      <c r="B167" t="s">
-        <v>167</v>
+      <c r="B167">
+        <v>52324</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="d">
         <v>2011-10-01</v>
       </c>
-      <c r="B168" t="s">
-        <v>168</v>
+      <c r="B168">
+        <v>58338</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="d">
         <v>2011-11-01</v>
       </c>
-      <c r="B169" t="s">
-        <v>169</v>
+      <c r="B169">
+        <v>56875</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="d">
         <v>2011-12-01</v>
       </c>
-      <c r="B170" t="s">
-        <v>170</v>
+      <c r="B170">
+        <v>56754</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="d">
         <v>2012-01-01</v>
       </c>
-      <c r="B171" t="s">
-        <v>171</v>
+      <c r="B171">
+        <v>63072</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="d">
         <v>2012-02-01</v>
       </c>
-      <c r="B172" t="s">
-        <v>173</v>
+      <c r="B172">
+        <v>65812</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="d">
         <v>2012-03-01</v>
       </c>
-      <c r="B173" t="s">
-        <v>174</v>
+      <c r="B173">
+        <v>64511</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="d">
         <v>2012-04-01</v>
       </c>
-      <c r="B174" t="s">
-        <v>175</v>
+      <c r="B174">
+        <v>61820</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="d">
         <v>2012-05-01</v>
       </c>
-      <c r="B175" t="s">
-        <v>176</v>
+      <c r="B175">
+        <v>54490</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="d">
         <v>2012-06-01</v>
       </c>
-      <c r="B176" t="s">
-        <v>177</v>
+      <c r="B176">
+        <v>54355</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="d">
         <v>2012-07-01</v>
       </c>
-      <c r="B177" t="s">
-        <v>178</v>
+      <c r="B177">
+        <v>56097</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="d">
         <v>2012-08-01</v>
       </c>
-      <c r="B178" t="s">
-        <v>179</v>
+      <c r="B178">
+        <v>57061</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="d">
         <v>2012-09-01</v>
       </c>
-      <c r="B179" t="s">
-        <v>180</v>
+      <c r="B179">
+        <v>59176</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="d">
         <v>2012-10-01</v>
       </c>
-      <c r="B180" t="s">
-        <v>181</v>
+      <c r="B180">
+        <v>57068</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="d">
         <v>2012-11-01</v>
       </c>
-      <c r="B181" t="s">
-        <v>182</v>
+      <c r="B181">
+        <v>57475</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="d">
         <v>2012-12-01</v>
       </c>
-      <c r="B182" t="s">
-        <v>183</v>
+      <c r="B182">
+        <v>60952</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="d">
         <v>2013-01-01</v>
       </c>
-      <c r="B183" t="s">
-        <v>184</v>
+      <c r="B183">
+        <v>59761</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="d">
         <v>2013-02-01</v>
       </c>
-      <c r="B184" t="s">
-        <v>185</v>
+      <c r="B184">
+        <v>57424</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="d">
         <v>2013-03-01</v>
       </c>
-      <c r="B185" t="s">
-        <v>186</v>
+      <c r="B185">
+        <v>56352</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="d">
         <v>2013-04-01</v>
       </c>
-      <c r="B186" t="s">
-        <v>187</v>
+      <c r="B186">
+        <v>55910</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="d">
         <v>2013-05-01</v>
       </c>
-      <c r="B187" t="s">
-        <v>188</v>
+      <c r="B187">
+        <v>53506</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="d">
         <v>2013-06-01</v>
       </c>
-      <c r="B188" t="s">
-        <v>189</v>
+      <c r="B188">
+        <v>47457</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="d">
         <v>2013-07-01</v>
       </c>
-      <c r="B189" t="s">
-        <v>190</v>
+      <c r="B189">
+        <v>48234</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="d">
         <v>2013-08-01</v>
       </c>
-      <c r="B190" t="s">
-        <v>191</v>
+      <c r="B190">
+        <v>50008</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="d">
         <v>2013-09-01</v>
       </c>
-      <c r="B191" t="s">
-        <v>192</v>
+      <c r="B191">
+        <v>52338</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="d">
         <v>2013-10-01</v>
       </c>
-      <c r="B192" t="s">
-        <v>193</v>
+      <c r="B192">
+        <v>54256</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="d">
         <v>2013-11-01</v>
       </c>
-      <c r="B193" t="s">
-        <v>194</v>
+      <c r="B193">
+        <v>52482</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="d">
         <v>2013-12-01</v>
       </c>
-      <c r="B194" t="s">
-        <v>195</v>
+      <c r="B194">
+        <v>51507</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="d">
         <v>2014-01-01</v>
       </c>
-      <c r="B195" t="s">
-        <v>196</v>
+      <c r="B195">
+        <v>47639</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="d">
         <v>2014-02-01</v>
       </c>
-      <c r="B196" t="s">
-        <v>197</v>
+      <c r="B196">
+        <v>47094</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="d">
         <v>2014-03-01</v>
       </c>
-      <c r="B197" t="s">
-        <v>198</v>
+      <c r="B197">
+        <v>50415</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="d">
         <v>2014-04-01</v>
       </c>
-      <c r="B198" t="s">
-        <v>199</v>
+      <c r="B198">
+        <v>51626</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="d">
         <v>2014-05-01</v>
       </c>
-      <c r="B199" t="s">
-        <v>200</v>
+      <c r="B199">
+        <v>51239</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="d">
         <v>2014-06-01</v>
       </c>
-      <c r="B200" t="s">
-        <v>201</v>
+      <c r="B200">
+        <v>53168</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="d">
         <v>2014-07-01</v>
       </c>
-      <c r="B201" t="s">
-        <v>202</v>
+      <c r="B201">
+        <v>55829</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="d">
         <v>2014-08-01</v>
       </c>
-      <c r="B202" t="s">
-        <v>203</v>
+      <c r="B202">
+        <v>61288</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="d">
         <v>2014-09-01</v>
       </c>
-      <c r="B203" t="s">
-        <v>204</v>
+      <c r="B203">
+        <v>54116</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="d">
         <v>2014-10-01</v>
       </c>
-      <c r="B204" t="s">
-        <v>205</v>
+      <c r="B204">
+        <v>54629</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="d">
         <v>2014-11-01</v>
       </c>
-      <c r="B205" t="s">
-        <v>206</v>
+      <c r="B205">
+        <v>54664</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="d">
         <v>2014-12-01</v>
       </c>
-      <c r="B206" t="s">
-        <v>207</v>
+      <c r="B206">
+        <v>50007</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="d">
         <v>2015-01-01</v>
       </c>
-      <c r="B207" t="s">
-        <v>208</v>
+      <c r="B207">
+        <v>46908</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="d">
         <v>2015-02-01</v>
       </c>
-      <c r="B208" t="s">
-        <v>209</v>
+      <c r="B208">
+        <v>51583</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="d">
         <v>2015-03-01</v>
       </c>
-      <c r="B209" t="s">
-        <v>210</v>
+      <c r="B209">
+        <v>51150</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="d">
         <v>2015-04-01</v>
       </c>
-      <c r="B210" t="s">
-        <v>211</v>
+      <c r="B210">
+        <v>56229</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="d">
         <v>2015-05-01</v>
       </c>
-      <c r="B211" t="s">
-        <v>212</v>
+      <c r="B211">
+        <v>52760</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="d">
         <v>2015-06-01</v>
       </c>
-      <c r="B212" t="s">
-        <v>213</v>
+      <c r="B212">
+        <v>53081</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="d">
         <v>2015-07-01</v>
       </c>
-      <c r="B213" t="s">
-        <v>214</v>
+      <c r="B213">
+        <v>50865</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="d">
         <v>2015-08-01</v>
       </c>
-      <c r="B214" t="s">
-        <v>215</v>
+      <c r="B214">
+        <v>46626</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="d">
         <v>2015-09-01</v>
       </c>
-      <c r="B215" t="s">
-        <v>216</v>
+      <c r="B215">
+        <v>45059</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="d">
         <v>2015-10-01</v>
       </c>
-      <c r="B216" t="s">
-        <v>217</v>
+      <c r="B216">
+        <v>45869</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="d">
         <v>2015-11-01</v>
       </c>
-      <c r="B217" t="s">
-        <v>218</v>
+      <c r="B217">
+        <v>45120</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="d">
         <v>2015-12-01</v>
       </c>
-      <c r="B218" t="s">
-        <v>219</v>
+      <c r="B218">
+        <v>43350</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="d">
         <v>2016-01-01</v>
       </c>
-      <c r="B219" t="s">
-        <v>220</v>
+      <c r="B219">
+        <v>40406</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="d">
         <v>2016-02-01</v>
       </c>
-      <c r="B220" t="s">
-        <v>221</v>
+      <c r="B220">
+        <v>42794</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="d">
         <v>2016-03-01</v>
       </c>
-      <c r="B221" t="s">
-        <v>222</v>
+      <c r="B221">
+        <v>50055</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="d">
         <v>2016-04-01</v>
       </c>
-      <c r="B222" t="s">
-        <v>223</v>
+      <c r="B222">
+        <v>53911</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="d">
         <v>2016-05-01</v>
       </c>
-      <c r="B223" t="s">
-        <v>224</v>
+      <c r="B223">
+        <v>48472</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="d">
         <v>2016-06-01</v>
       </c>
-      <c r="B224" t="s">
-        <v>225</v>
+      <c r="B224">
+        <v>51527</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="d">
         <v>2016-07-01</v>
       </c>
-      <c r="B225" t="s">
-        <v>226</v>
+      <c r="B225">
+        <v>57308</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="d">
         <v>2016-08-01</v>
       </c>
-      <c r="B226" t="s">
-        <v>227</v>
+      <c r="B226">
+        <v>57901</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="d">
         <v>2016-09-01</v>
       </c>
-      <c r="B227" t="s">
-        <v>228</v>
+      <c r="B227">
+        <v>58367</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="d">
         <v>2016-10-01</v>
       </c>
-      <c r="B228" t="s">
-        <v>229</v>
+      <c r="B228">
+        <v>64925</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="d">
         <v>2016-11-01</v>
       </c>
-      <c r="B229" t="s">
-        <v>230</v>
+      <c r="B229">
+        <v>61906</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="d">
         <v>2016-12-01</v>
       </c>
-      <c r="B230" t="s">
-        <v>231</v>
+      <c r="B230">
+        <v>60227</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="d">
         <v>2017-01-01</v>
       </c>
-      <c r="B231" t="s">
-        <v>232</v>
+      <c r="B231">
+        <v>64671</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="d">
         <v>2017-02-01</v>
       </c>
-      <c r="B232" t="s">
-        <v>172</v>
+      <c r="B232">
+        <v>66662</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="d">
         <v>2017-03-01</v>
       </c>
-      <c r="B233" t="s">
-        <v>233</v>
+      <c r="B233">
+        <v>64984</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="d">
         <v>2017-04-01</v>
       </c>
-      <c r="B234" t="s">
-        <v>234</v>
+      <c r="B234">
+        <v>65403</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="d">
         <v>2017-05-01</v>
       </c>
-      <c r="B235" t="s">
-        <v>235</v>
+      <c r="B235">
+        <v>62711</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="d">
         <v>2017-06-01</v>
       </c>
-      <c r="B236" t="s">
-        <v>236</v>
+      <c r="B236">
+        <v>62900</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="d">
         <v>2017-07-01</v>
       </c>
-      <c r="B237" t="s">
-        <v>237</v>
+      <c r="B237">
+        <v>65920</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="d">
         <v>2017-08-01</v>
       </c>
-      <c r="B238" t="s">
-        <v>238</v>
+      <c r="B238">
+        <v>70835</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="d">
         <v>2017-09-01</v>
       </c>
-      <c r="B239" t="s">
-        <v>239</v>
+      <c r="B239">
+        <v>74294</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="d">
         <v>2017-10-01</v>
       </c>
-      <c r="B240" t="s">
-        <v>240</v>
+      <c r="B240">
+        <v>74308</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="d">
         <v>2017-11-01</v>
       </c>
-      <c r="B241" t="s">
-        <v>241</v>
+      <c r="B241">
+        <v>71971</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="d">
         <v>2017-12-01</v>
       </c>
-      <c r="B242" t="s">
-        <v>242</v>
+      <c r="B242">
+        <v>76402</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="d">
         <v>2018-01-01</v>
       </c>
-      <c r="B243" t="s">
-        <v>243</v>
+      <c r="B243">
+        <v>84913</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="d">
         <v>2018-02-01</v>
       </c>
-      <c r="B244" t="s">
-        <v>244</v>
+      <c r="B244">
+        <v>85481</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="d">
         <v>2018-03-01</v>
       </c>
-      <c r="B245" t="s">
-        <v>245</v>
+      <c r="B245">
+        <v>85366</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="d">
         <v>2018-04-01</v>
       </c>
-      <c r="B246" t="s">
-        <v>246</v>
+      <c r="B246">
+        <v>86115</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="d">
         <v>2018-05-01</v>
       </c>
-      <c r="B247" t="s">
-        <v>247</v>
+      <c r="B247">
+        <v>76754</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="d">
         <v>2018-06-01</v>
       </c>
-      <c r="B248" t="s">
-        <v>248</v>
+      <c r="B248">
+        <v>72763</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="d">
         <v>2018-07-01</v>
       </c>
-      <c r="B249" t="s">
-        <v>249</v>
+      <c r="B249">
+        <v>79220</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="d">
         <v>2018-08-01</v>
       </c>
-      <c r="B250" t="s">
-        <v>250</v>
+      <c r="B250">
+        <v>76678</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="d">
         <v>2018-09-01</v>
       </c>
-      <c r="B251" t="s">
-        <v>251</v>
+      <c r="B251">
+        <v>79342</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="d">
         <v>2018-10-01</v>
       </c>
-      <c r="B252" t="s">
-        <v>252</v>
+      <c r="B252">
+        <v>87424</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="d">
         <v>2018-11-01</v>
       </c>
-      <c r="B253" t="s">
-        <v>253</v>
+      <c r="B253">
+        <v>89504</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="d">
         <v>2018-12-01</v>
       </c>
-      <c r="B254" t="s">
-        <v>254</v>
+      <c r="B254">
+        <v>87887</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="d">
         <v>2019-01-01</v>
       </c>
-      <c r="B255" t="s">
-        <v>255</v>
+      <c r="B255">
+        <v>97394</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="d">
         <v>2019-02-01</v>
       </c>
-      <c r="B256" t="s">
-        <v>256</v>
+      <c r="B256">
+        <v>95584</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="d">
         <v>2019-03-01</v>
       </c>
-      <c r="B257" t="s">
-        <v>257</v>
+      <c r="B257">
+        <v>95415</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="d">
         <v>2019-04-01</v>
       </c>
-      <c r="B258" t="s">
-        <v>258</v>
+      <c r="B258">
+        <v>96353</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="d">
         <v>2019-05-01</v>
       </c>
-      <c r="B259" t="s">
-        <v>259</v>
+      <c r="B259">
+        <v>97030</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="d">
         <v>2019-06-01</v>
       </c>
-      <c r="B260" t="s">
-        <v>260</v>
+      <c r="B260">
+        <v>100967</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="d">
         <v>2019-07-01</v>
       </c>
-      <c r="B261" t="s">
-        <v>261</v>
+      <c r="B261">
+        <v>101812</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="d">
         <v>2019-08-01</v>
       </c>
-      <c r="B262" t="s">
-        <v>262</v>
+      <c r="B262">
+        <v>101135</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="d">
         <v>2019-09-01</v>
       </c>
-      <c r="B263" t="s">
-        <v>263</v>
+      <c r="B263">
+        <v>104745</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="d">
         <v>2019-10-01</v>
       </c>
-      <c r="B264" t="s">
-        <v>264</v>
+      <c r="B264">
+        <v>107220</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="d">
         <v>2019-11-01</v>
       </c>
-      <c r="B265" t="s">
-        <v>265</v>
+      <c r="B265">
+        <v>108233</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="d">
         <v>2019-12-01</v>
       </c>
-      <c r="B266" t="s">
-        <v>266</v>
+      <c r="B266">
+        <v>115645</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="d">
         <v>2020-01-01</v>
       </c>
-      <c r="B267" t="s">
-        <v>267</v>
+      <c r="B267">
+        <v>113761</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="d">
         <v>2020-02-01</v>
       </c>
-      <c r="B268" t="s">
-        <v>268</v>
+      <c r="B268">
+        <v>104172</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="d">
         <v>2020-03-01</v>
       </c>
-      <c r="B269" t="s">
-        <v>269</v>
+      <c r="B269">
+        <v>73020</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="d">
         <v>2020-04-01</v>
       </c>
-      <c r="B270" t="s">
-        <v>270</v>
+      <c r="B270">
+        <v>80506</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="d">
         <v>2020-05-01</v>
       </c>
-      <c r="B271" t="s">
-        <v>271</v>
+      <c r="B271">
+        <v>87403</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="d">
         <v>2020-06-01</v>
       </c>
-      <c r="B272" t="s">
-        <v>272</v>
+      <c r="B272">
+        <v>95056</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="d">
         <v>2020-07-01</v>
       </c>
-      <c r="B273" t="s">
-        <v>273</v>
+      <c r="B273">
+        <v>102912</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="d">
         <v>2020-08-01</v>
       </c>
-      <c r="B274" t="s">
-        <v>274</v>
+      <c r="B274">
+        <v>99369</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="d">
         <v>2020-09-01</v>
       </c>
-      <c r="B275" t="s">
-        <v>275</v>
+      <c r="B275">
+        <v>94603</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="d">
         <v>2020-10-01</v>
       </c>
-      <c r="B276" t="s">
-        <v>276</v>
+      <c r="B276">
+        <v>93952</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="d">
         <v>2020-11-01</v>
       </c>
-      <c r="B277" t="s">
-        <v>277</v>
+      <c r="B277">
+        <v>108888</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="d">
         <v>2020-12-01</v>
       </c>
-      <c r="B278" t="s">
-        <v>278</v>
+      <c r="B278">
+        <v>119306</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="d">
         <v>2021-01-01</v>
       </c>
-      <c r="B279" t="s">
-        <v>279</v>
+      <c r="B279">
+        <v>116007</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="d">
         <v>2021-02-01</v>
       </c>
-      <c r="B280" t="s">
-        <v>280</v>
+      <c r="B280">
+        <v>110035</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="d">
         <v>2021-03-01</v>
       </c>
-      <c r="B281" t="s">
-        <v>281</v>
+      <c r="B281">
+        <v>116634</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="d">
         <v>2021-04-01</v>
       </c>
-      <c r="B282" t="s">
-        <v>282</v>
+      <c r="B282">
+        <v>118894</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="d">
         <v>2021-05-01</v>
       </c>
-      <c r="B283" t="s">
-        <v>283</v>
+      <c r="B283">
+        <v>126216</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="d">
         <v>2021-06-01</v>
       </c>
-      <c r="B284" t="s">
-        <v>284</v>
+      <c r="B284">
+        <v>126802</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="d">
         <v>2021-07-01</v>
       </c>
-      <c r="B285" t="s">
-        <v>285</v>
+      <c r="B285">
+        <v>121801</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="d">
         <v>2021-08-01</v>
       </c>
-      <c r="B286" t="s">
-        <v>286</v>
+      <c r="B286">
+        <v>118781</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="d">
         <v>2021-09-01</v>
       </c>
-      <c r="B287" t="s">
-        <v>287</v>
+      <c r="B287">
+        <v>110979</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="d">
         <v>2021-10-01</v>
       </c>
-      <c r="B288" t="s">
-        <v>288</v>
+      <c r="B288">
+        <v>103501</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="d">
         <v>2021-11-01</v>
       </c>
-      <c r="B289" t="s">
-        <v>289</v>
+      <c r="B289">
+        <v>101915</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="d">
         <v>2021-12-01</v>
       </c>
-      <c r="B290" t="s">
-        <v>290</v>
+      <c r="B290">
+        <v>104822</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="d">
         <v>2022-01-01</v>
       </c>
-      <c r="B291" t="s">
-        <v>291</v>
+      <c r="B291">
+        <v>112388</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="d">
         <v>2022-02-01</v>
       </c>
-      <c r="B292" t="s">
-        <v>292</v>
+      <c r="B292">
+        <v>113142</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="d">
         <v>2022-03-01</v>
       </c>
-      <c r="B293" t="s">
-        <v>293</v>
+      <c r="B293">
+        <v>119999</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="d">
         <v>2022-04-01</v>
       </c>
-      <c r="B294" t="s">
-        <v>294</v>
+      <c r="B294">
+        <v>107876</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="d">
         <v>2022-05-01</v>
       </c>
-      <c r="B295" t="s">
-        <v>295</v>
+      <c r="B295">
+        <v>111351</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="d">
         <v>2022-06-01</v>
       </c>
-      <c r="B296" t="s">
-        <v>296</v>
+      <c r="B296">
+        <v>98542</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="d">
         <v>2022-07-01</v>
       </c>
-      <c r="B297" t="s">
-        <v>297</v>
+      <c r="B297">
+        <v>103165</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="d">
         <v>2022-08-01</v>
       </c>
-      <c r="B298" t="s">
-        <v>298</v>
+      <c r="B298">
+        <v>109523</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="d">
         <v>2022-09-01</v>
       </c>
-      <c r="B299" t="s">
-        <v>299</v>
+      <c r="B299">
+        <v>110037</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="d">
         <v>2022-10-01</v>
       </c>
-      <c r="B300" t="s">
-        <v>300</v>
+      <c r="B300">
+        <v>116037</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="d">
         <v>2022-11-01</v>
       </c>
-      <c r="B301" t="s">
-        <v>301</v>
+      <c r="B301">
+        <v>112486</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="d">
         <v>2022-12-01</v>
       </c>
-      <c r="B302" t="s">
-        <v>302</v>
+      <c r="B302">
+        <v>110031</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="d">
         <v>2023-01-01</v>
       </c>
-      <c r="B303" t="s">
-        <v>303</v>
+      <c r="B303">
+        <v>113532</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="d">
         <v>2023-02-01</v>
       </c>
-      <c r="B304" t="s">
-        <v>304</v>
+      <c r="B304">
+        <v>104932</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="d">
         <v>2023-03-01</v>
       </c>
-      <c r="B305" t="s">
-        <v>305</v>
+      <c r="B305">
+        <v>101793</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="d">
         <v>2023-03-29</v>
       </c>
-      <c r="B306" t="s">
-        <v>306</v>
+      <c r="B306">
+        <v>101792.523438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>